<commit_message>
Update excel inserendo i modelli di Paolo
</commit_message>
<xml_diff>
--- a/Modelli testati.xlsx
+++ b/Modelli testati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Marco\Universita\Magistrale\FVAB\prog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elepa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD25590-CCA9-4C49-B55F-8522D51A4B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF1648E-EC91-4B74-82F4-E0C26F7E5977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA2C581A-40E4-4BB1-8846-957B366FFFDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{EA2C581A-40E4-4BB1-8846-957B366FFFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="149">
   <si>
     <t>🔹 Modelli principali (Stable Diffusion 2.x / 3.x / XL)</t>
   </si>
@@ -490,12 +490,21 @@
   <si>
     <t>🔹 Realistic Vision (EXTRA)</t>
   </si>
+  <si>
+    <t>Errore di autorizzazione: il modello è privato, serve autenticarsi su Hugging Face.</t>
+  </si>
+  <si>
+    <t>Errore di risorsa: il modello non esiste sull'URL indicato.</t>
+  </si>
+  <si>
+    <t>Il modello tende sempre ad avere crash non previsti</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,13 +529,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
@@ -541,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +553,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -742,6 +756,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -751,6 +800,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,52 +812,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1145,22 +1167,22 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="D1:E1"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="122.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="49.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="122.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1172,919 +1194,900 @@
       <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="26" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="F16" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="11" t="s">
+      <c r="E34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="E42" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="24"/>
+      <c r="C45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="24"/>
+      <c r="C47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="24"/>
+      <c r="C48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="E49" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="E50" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="24"/>
+      <c r="C51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="24"/>
+      <c r="C52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="24"/>
+      <c r="C54" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F37" s="11"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" s="11"/>
-    </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F43" s="11"/>
-    </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F44" s="11"/>
-    </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="F45" s="11"/>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F46" s="11"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F49" s="11"/>
-    </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F50" s="11"/>
-    </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51" s="11"/>
-    </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F52" s="11"/>
-    </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F53" s="11"/>
-    </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F54" s="11"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="29" t="s">
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="11" t="s">
+      <c r="B56" s="21"/>
+      <c r="C56" s="1" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="B55:B56"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="B33:B34"/>
@@ -2096,8 +2099,6 @@
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="F2:F6"/>
-    <mergeCell ref="B43:B54"/>
-    <mergeCell ref="B55:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update paolo (colore celle)
</commit_message>
<xml_diff>
--- a/Modelli testati.xlsx
+++ b/Modelli testati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elepa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF1648E-EC91-4B74-82F4-E0C26F7E5977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188DFD10-8343-4A9E-8E2F-50FD464B71F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{EA2C581A-40E4-4BB1-8846-957B366FFFDA}"/>
   </bookViews>
@@ -543,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,6 +568,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -745,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -791,43 +797,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1167,7 +1176,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="16" x14ac:dyDescent="0.35"/>
@@ -1202,7 +1211,7 @@
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1214,7 +1223,7 @@
       <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="30" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1222,7 +1231,7 @@
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
@@ -1232,13 +1241,13 @@
       <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1248,13 +1257,13 @@
       <c r="E4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1264,13 +1273,13 @@
       <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1280,13 +1289,13 @@
       <c r="E6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1301,7 +1310,7 @@
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1316,7 +1325,7 @@
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1331,7 +1340,7 @@
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1346,7 +1355,7 @@
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1373,7 @@
       <c r="A12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="20"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
@@ -1379,10 +1388,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
@@ -1394,10 +1403,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1409,10 +1418,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1424,10 +1433,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
@@ -1442,10 +1451,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1462,10 +1471,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1480,10 +1489,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1498,10 +1507,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1516,10 +1525,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="21"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="1" t="s">
         <v>68</v>
       </c>
@@ -1534,10 +1543,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1551,10 +1560,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
@@ -1569,7 +1578,7 @@
       <c r="A24" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="1" t="s">
         <v>73</v>
       </c>
@@ -1659,7 +1668,7 @@
       <c r="E29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="28" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1667,7 +1676,7 @@
       <c r="A30" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="25"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="1" t="s">
         <v>78</v>
       </c>
@@ -1677,7 +1686,7 @@
       <c r="E30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="22"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
@@ -1695,7 +1704,7 @@
       <c r="E31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="28" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1703,7 +1712,7 @@
       <c r="A32" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="25"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1713,7 +1722,7 @@
       <c r="E32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
@@ -1731,7 +1740,7 @@
       <c r="E33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="28" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1749,13 +1758,13 @@
       <c r="E34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F34" s="22"/>
+      <c r="F34" s="28"/>
     </row>
     <row r="35" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="25" t="s">
         <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1772,7 +1781,7 @@
       <c r="A36" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="20"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="1" t="s">
         <v>102</v>
       </c>
@@ -1787,7 +1796,7 @@
       <c r="A37" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="1" t="s">
         <v>102</v>
       </c>
@@ -1802,7 +1811,7 @@
       <c r="A38" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="20"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="1" t="s">
         <v>102</v>
       </c>
@@ -1817,7 +1826,7 @@
       <c r="A39" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="20"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="1" t="s">
         <v>102</v>
       </c>
@@ -1832,7 +1841,7 @@
       <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="20"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="1" t="s">
         <v>102</v>
       </c>
@@ -1847,7 +1856,7 @@
       <c r="A41" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="1" t="s">
         <v>102</v>
       </c>
@@ -1862,7 +1871,7 @@
       <c r="A42" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="1" t="s">
         <v>102</v>
       </c>
@@ -2059,7 +2068,7 @@
       <c r="A55" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="25" t="s">
         <v>145</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2079,26 +2088,26 @@
       <c r="A56" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B56" s="21"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="1" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B43:B54"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B2:B16"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="B31:B32"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F2:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update modelli Mattia + update xlsx modelli
</commit_message>
<xml_diff>
--- a/Modelli testati.xlsx
+++ b/Modelli testati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Marco\Universita\Magistrale\FVAB\prog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattia\Desktop\REP\FVAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD25590-CCA9-4C49-B55F-8522D51A4B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6769DD9A-236C-42A0-8CCD-66D287A2CB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA2C581A-40E4-4BB1-8846-957B366FFFDA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA2C581A-40E4-4BB1-8846-957B366FFFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="148">
   <si>
     <t>🔹 Modelli principali (Stable Diffusion 2.x / 3.x / XL)</t>
   </si>
@@ -490,12 +490,18 @@
   <si>
     <t>🔹 Realistic Vision (EXTRA)</t>
   </si>
+  <si>
+    <t>Velocità generazione accettabile. Risultati non ottimali. Richiederebbe fine-tuning</t>
+  </si>
+  <si>
+    <t>Oneroso in termini computazionali.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,13 +520,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -731,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -742,6 +741,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -751,6 +785,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,53 +797,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,14 +1139,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728E2DCA-7DDA-4D3C-8A56-4C16485960FE}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1160,7 +1155,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1172,902 +1167,875 @@
       <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="26" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="27" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="21"/>
+      <c r="C24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="11" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="11" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="24"/>
+      <c r="C29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="11" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="22" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="11" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="11" t="s">
+      <c r="D33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="22" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="11" t="s">
+      <c r="D35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="11" t="s">
+      <c r="B36" s="20"/>
+      <c r="C36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="11" t="s">
+      <c r="D36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="20"/>
+      <c r="C37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="11" t="s">
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="11" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="11" t="s">
+      <c r="B39" s="20"/>
+      <c r="C39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="11" t="s">
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="11" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="11" t="s">
+      <c r="D40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="11" t="s">
+      <c r="B41" s="20"/>
+      <c r="C41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="11" t="s">
+      <c r="D41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="11" t="s">
+      <c r="B42" s="21"/>
+      <c r="C42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="11" t="s">
+      <c r="B44" s="24"/>
+      <c r="C44" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="11" t="s">
+      <c r="B45" s="24"/>
+      <c r="C45" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="11" t="s">
+      <c r="B46" s="24"/>
+      <c r="C46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E46" s="11" t="s">
+      <c r="D46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="11" t="s">
+      <c r="B47" s="24"/>
+      <c r="C47" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="11" t="s">
+      <c r="D47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="11" t="s">
+      <c r="B48" s="24"/>
+      <c r="C48" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="11" t="s">
+      <c r="D48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="11" t="s">
+      <c r="B49" s="24"/>
+      <c r="C49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="11" t="s">
+      <c r="B50" s="24"/>
+      <c r="C50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="11" t="s">
+      <c r="B51" s="24"/>
+      <c r="C51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="11" t="s">
+      <c r="B52" s="24"/>
+      <c r="C52" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="11" t="s">
+      <c r="B53" s="24"/>
+      <c r="C53" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="11" t="s">
+      <c r="B54" s="24"/>
+      <c r="C54" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D54" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F55" s="1" t="s">
@@ -2075,16 +2043,18 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="11" t="s">
+      <c r="B56" s="21"/>
+      <c r="C56" s="1" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="B55:B56"/>
     <mergeCell ref="B35:B42"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="B33:B34"/>
@@ -2096,10 +2066,8 @@
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="F2:F6"/>
-    <mergeCell ref="B43:B54"/>
-    <mergeCell ref="B55:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>